<commit_message>
Modified files for constant height
</commit_message>
<xml_diff>
--- a/data/constant_height_profile.xlsx
+++ b/data/constant_height_profile.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Feedrate (mm/s)</t>
+          <t>Average Height (mm)</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
         <v>12.48907317843619</v>
       </c>
       <c r="E2" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="3">
@@ -491,7 +491,7 @@
         <v>12.49697800065648</v>
       </c>
       <c r="E3" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="4">
@@ -508,7 +508,7 @@
         <v>12.4916898647475</v>
       </c>
       <c r="E4" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
         <v>12.4849265194308</v>
       </c>
       <c r="E5" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>12.50013976411079</v>
       </c>
       <c r="E6" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="7">
@@ -559,7 +559,7 @@
         <v>12.5103033348664</v>
       </c>
       <c r="E7" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="8">
@@ -576,7 +576,7 @@
         <v>12.50667611440884</v>
       </c>
       <c r="E8" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="9">
@@ -593,7 +593,7 @@
         <v>12.50648265903559</v>
       </c>
       <c r="E9" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="10">
@@ -610,7 +610,7 @@
         <v>12.50323403391101</v>
       </c>
       <c r="E10" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="11">
@@ -627,7 +627,7 @@
         <v>12.50739057240202</v>
       </c>
       <c r="E11" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="12">
@@ -644,7 +644,7 @@
         <v>12.49542880188019</v>
       </c>
       <c r="E12" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="13">
@@ -661,7 +661,7 @@
         <v>12.49030407982103</v>
       </c>
       <c r="E13" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="14">
@@ -678,7 +678,7 @@
         <v>12.49334790234708</v>
       </c>
       <c r="E14" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="15">
@@ -695,7 +695,7 @@
         <v>12.48690063493668</v>
       </c>
       <c r="E15" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="16">
@@ -712,7 +712,7 @@
         <v>12.4906429993539</v>
       </c>
       <c r="E16" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="17">
@@ -729,7 +729,7 @@
         <v>12.49888953315865</v>
       </c>
       <c r="E17" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="18">
@@ -746,7 +746,7 @@
         <v>12.49984764356134</v>
       </c>
       <c r="E18" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="19">
@@ -763,7 +763,7 @@
         <v>12.50590818844525</v>
       </c>
       <c r="E19" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="20">
@@ -780,7 +780,7 @@
         <v>12.49606444019295</v>
       </c>
       <c r="E20" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="21">
@@ -797,7 +797,7 @@
         <v>12.5002618148661</v>
       </c>
       <c r="E21" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="22">
@@ -814,7 +814,7 @@
         <v>12.50346059907482</v>
       </c>
       <c r="E22" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="23">
@@ -831,7 +831,7 @@
         <v>12.50689766921612</v>
       </c>
       <c r="E23" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="24">
@@ -848,7 +848,7 @@
         <v>12.49159411858025</v>
       </c>
       <c r="E24" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="25">
@@ -865,7 +865,7 @@
         <v>12.49565663763035</v>
       </c>
       <c r="E25" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="26">
@@ -882,7 +882,7 @@
         <v>12.50084315289363</v>
       </c>
       <c r="E26" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="27">
@@ -899,7 +899,7 @@
         <v>12.50425801951379</v>
       </c>
       <c r="E27" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="28">
@@ -916,7 +916,7 @@
         <v>12.49835094976859</v>
       </c>
       <c r="E28" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="29">
@@ -933,7 +933,7 @@
         <v>12.49654753373083</v>
       </c>
       <c r="E29" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="30">
@@ -950,7 +950,7 @@
         <v>12.49530321835534</v>
       </c>
       <c r="E30" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="31">
@@ -967,7 +967,7 @@
         <v>12.4946090027955</v>
       </c>
       <c r="E31" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="32">
@@ -984,7 +984,7 @@
         <v>12.47503793060935</v>
       </c>
       <c r="E32" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="33">
@@ -1001,7 +1001,7 @@
         <v>12.48553717050293</v>
       </c>
       <c r="E33" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="34">
@@ -1018,7 +1018,7 @@
         <v>12.49553928979014</v>
       </c>
       <c r="E34" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="35">
@@ -1035,7 +1035,7 @@
         <v>12.50412224432166</v>
       </c>
       <c r="E35" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="36">
@@ -1052,7 +1052,7 @@
         <v>12.49941338155498</v>
       </c>
       <c r="E36" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="37">
@@ -1069,7 +1069,7 @@
         <v>12.48836724195577</v>
       </c>
       <c r="E37" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="38">
@@ -1086,7 +1086,7 @@
         <v>12.4931918363365</v>
       </c>
       <c r="E38" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="39">
@@ -1103,7 +1103,7 @@
         <v>12.50160947837563</v>
       </c>
       <c r="E39" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="40">
@@ -1120,7 +1120,7 @@
         <v>12.50810664839344</v>
       </c>
       <c r="E40" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="41">
@@ -1137,7 +1137,7 @@
         <v>12.49977642985315</v>
       </c>
       <c r="E41" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="42">
@@ -1154,7 +1154,7 @@
         <v>12.49286353162554</v>
       </c>
       <c r="E42" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="43">
@@ -1171,7 +1171,7 @@
         <v>12.49238507788027</v>
       </c>
       <c r="E43" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="44">
@@ -1188,7 +1188,7 @@
         <v>12.49910735051071</v>
       </c>
       <c r="E44" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="45">
@@ -1205,7 +1205,7 @@
         <v>12.50102462004743</v>
       </c>
       <c r="E45" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="46">
@@ -1222,7 +1222,7 @@
         <v>12.5004257124665</v>
       </c>
       <c r="E46" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="47">
@@ -1239,7 +1239,7 @@
         <v>12.49903817581628</v>
       </c>
       <c r="E47" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="48">
@@ -1256,7 +1256,7 @@
         <v>12.49112619916742</v>
       </c>
       <c r="E48" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="49">
@@ -1273,7 +1273,7 @@
         <v>12.49530268040168</v>
       </c>
       <c r="E49" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="50">
@@ -1290,7 +1290,7 @@
         <v>12.49181955028149</v>
       </c>
       <c r="E50" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="51">
@@ -1307,7 +1307,7 @@
         <v>12.49457827983889</v>
       </c>
       <c r="E51" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="52">
@@ -1324,7 +1324,7 @@
         <v>12.49702157032008</v>
       </c>
       <c r="E52" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="53">
@@ -1341,7 +1341,7 @@
         <v>12.49303708517217</v>
       </c>
       <c r="E53" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="54">
@@ -1358,7 +1358,7 @@
         <v>12.50402751522788</v>
       </c>
       <c r="E54" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="55">
@@ -1375,7 +1375,7 @@
         <v>12.50745673724548</v>
       </c>
       <c r="E55" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="56">
@@ -1392,7 +1392,7 @@
         <v>12.51095066566723</v>
       </c>
       <c r="E56" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="57">
@@ -1409,7 +1409,7 @@
         <v>12.51287702338761</v>
       </c>
       <c r="E57" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="58">
@@ -1426,7 +1426,7 @@
         <v>12.50953643489349</v>
       </c>
       <c r="E58" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="59">
@@ -1443,7 +1443,7 @@
         <v>12.48824783620327</v>
       </c>
       <c r="E59" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="60">
@@ -1460,7 +1460,7 @@
         <v>12.49735017343991</v>
       </c>
       <c r="E60" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="61">
@@ -1477,7 +1477,7 @@
         <v>12.49296816040709</v>
       </c>
       <c r="E61" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="62">
@@ -1494,7 +1494,7 @@
         <v>12.50525247095839</v>
       </c>
       <c r="E62" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="63">
@@ -1511,7 +1511,7 @@
         <v>12.50865345378959</v>
       </c>
       <c r="E63" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="64">
@@ -1528,7 +1528,7 @@
         <v>12.5042714517277</v>
       </c>
       <c r="E64" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="65">
@@ -1545,7 +1545,7 @@
         <v>12.49641462195135</v>
       </c>
       <c r="E65" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="66">
@@ -1562,7 +1562,7 @@
         <v>12.49189525935506</v>
       </c>
       <c r="E66" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="67">
@@ -1579,7 +1579,7 @@
         <v>12.48918041548294</v>
       </c>
       <c r="E67" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="68">
@@ -1596,7 +1596,7 @@
         <v>12.49508451997021</v>
       </c>
       <c r="E68" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="69">
@@ -1613,7 +1613,7 @@
         <v>12.5010139574481</v>
       </c>
       <c r="E69" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="70">
@@ -1630,7 +1630,7 @@
         <v>12.49440665301461</v>
       </c>
       <c r="E70" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="71">
@@ -1647,7 +1647,7 @@
         <v>12.49784391772483</v>
       </c>
       <c r="E71" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="72">
@@ -1664,7 +1664,7 @@
         <v>12.50703876120208</v>
       </c>
       <c r="E72" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="73">
@@ -1681,7 +1681,7 @@
         <v>12.51379173557025</v>
       </c>
       <c r="E73" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="74">
@@ -1698,7 +1698,7 @@
         <v>12.51681524429828</v>
       </c>
       <c r="E74" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="75">
@@ -1715,7 +1715,7 @@
         <v>12.50357995004978</v>
       </c>
       <c r="E75" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="76">
@@ -1732,7 +1732,7 @@
         <v>12.50114700267057</v>
       </c>
       <c r="E76" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="77">
@@ -1749,7 +1749,7 @@
         <v>12.49400204883098</v>
       </c>
       <c r="E77" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="78">
@@ -1766,7 +1766,7 @@
         <v>12.49889230682842</v>
       </c>
       <c r="E78" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="79">
@@ -1783,7 +1783,7 @@
         <v>12.50104542132216</v>
       </c>
       <c r="E79" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="80">
@@ -1800,7 +1800,7 @@
         <v>12.49469386502821</v>
       </c>
       <c r="E80" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="81">
@@ -1817,7 +1817,7 @@
         <v>12.49871011534857</v>
       </c>
       <c r="E81" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="82">
@@ -1834,7 +1834,7 @@
         <v>12.49726333138935</v>
       </c>
       <c r="E82" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="83">
@@ -1851,7 +1851,7 @@
         <v>12.50249182863689</v>
       </c>
       <c r="E83" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="84">
@@ -1868,7 +1868,7 @@
         <v>12.50548959552697</v>
       </c>
       <c r="E84" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="85">
@@ -1885,7 +1885,7 @@
         <v>12.50900167093847</v>
       </c>
       <c r="E85" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="86">
@@ -1902,7 +1902,7 @@
         <v>12.51369498083013</v>
       </c>
       <c r="E86" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="87">
@@ -1919,7 +1919,7 @@
         <v>12.50312085906486</v>
       </c>
       <c r="E87" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="88">
@@ -1936,7 +1936,7 @@
         <v>12.50549380573058</v>
       </c>
       <c r="E88" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="89">
@@ -1953,7 +1953,7 @@
         <v>12.50430912176548</v>
       </c>
       <c r="E89" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="90">
@@ -1970,7 +1970,7 @@
         <v>12.49761930370601</v>
       </c>
       <c r="E90" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="91">
@@ -1987,7 +1987,7 @@
         <v>12.49535778250788</v>
       </c>
       <c r="E91" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="92">
@@ -2004,7 +2004,7 @@
         <v>12.49199411654976</v>
       </c>
       <c r="E92" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="93">
@@ -2021,7 +2021,7 @@
         <v>12.49563677466067</v>
       </c>
       <c r="E93" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="94">
@@ -2038,7 +2038,7 @@
         <v>12.50073162073406</v>
       </c>
       <c r="E94" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="95">
@@ -2055,7 +2055,7 @@
         <v>12.50454184268507</v>
       </c>
       <c r="E95" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="96">
@@ -2072,7 +2072,7 @@
         <v>12.51335462136347</v>
       </c>
       <c r="E96" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="97">
@@ -2089,7 +2089,7 @@
         <v>12.51989378336089</v>
       </c>
       <c r="E97" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="98">
@@ -2106,7 +2106,7 @@
         <v>12.5233057120509</v>
       </c>
       <c r="E98" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="99">
@@ -2123,7 +2123,7 @@
         <v>12.52315919408311</v>
       </c>
       <c r="E99" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="100">
@@ -2140,7 +2140,7 @@
         <v>12.50599252578233</v>
       </c>
       <c r="E100" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
     <row r="101">
@@ -2157,7 +2157,7 @@
         <v>12.50995734223904</v>
       </c>
       <c r="E101" t="n">
-        <v>46</v>
+        <v>2.060321760617581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified files for better r2 score
</commit_message>
<xml_diff>
--- a/data/constant_height_profile.xlsx
+++ b/data/constant_height_profile.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.036458738039161</v>
+        <v>2.095160230104522</v>
       </c>
       <c r="C2" t="n">
-        <v>5.010175062079751</v>
+        <v>5.005965860545533</v>
       </c>
       <c r="D2" t="n">
-        <v>19.70610503724785</v>
+        <v>18.00357951632732</v>
       </c>
       <c r="E2" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1.855849738238642</v>
+        <v>1.886232637392391</v>
       </c>
       <c r="C3" t="n">
-        <v>5.019205512069777</v>
+        <v>5.01641224018114</v>
       </c>
       <c r="D3" t="n">
-        <v>19.71152330724187</v>
+        <v>18.00984734410869</v>
       </c>
       <c r="E3" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.217750419359809</v>
+        <v>2.19309545946011</v>
       </c>
       <c r="C4" t="n">
-        <v>5.001110478013719</v>
+        <v>5.001069099077753</v>
       </c>
       <c r="D4" t="n">
-        <v>19.70066628680823</v>
+        <v>18.00064145944665</v>
       </c>
       <c r="E4" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2.510207402309924</v>
+        <v>2.473148346168887</v>
       </c>
       <c r="C5" t="n">
-        <v>4.986487628866213</v>
+        <v>4.987066454742314</v>
       </c>
       <c r="D5" t="n">
-        <v>19.69189257731973</v>
+        <v>17.99223987284539</v>
       </c>
       <c r="E5" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2.026062968455622</v>
+        <v>1.986185746177197</v>
       </c>
       <c r="C6" t="n">
-        <v>5.010694850558928</v>
+        <v>5.011414584741899</v>
       </c>
       <c r="D6" t="n">
-        <v>19.70641691033536</v>
+        <v>18.00684875084514</v>
       </c>
       <c r="E6" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +550,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1.715200961139949</v>
+        <v>1.672671793337828</v>
       </c>
       <c r="C7" t="n">
-        <v>5.026237950924712</v>
+        <v>5.027090282383868</v>
       </c>
       <c r="D7" t="n">
-        <v>19.71574277055483</v>
+        <v>18.01625416943032</v>
       </c>
       <c r="E7" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +567,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.888424529386958</v>
+        <v>1.842194708816258</v>
       </c>
       <c r="C8" t="n">
-        <v>5.017576772512362</v>
+        <v>5.018614136609946</v>
       </c>
       <c r="D8" t="n">
-        <v>19.71054606350742</v>
+        <v>18.01116848196597</v>
       </c>
       <c r="E8" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="9">
@@ -584,16 +584,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>1.91345645730348</v>
+        <v>1.866815088720299</v>
       </c>
       <c r="C9" t="n">
-        <v>5.016325176116536</v>
+        <v>5.017383117614744</v>
       </c>
       <c r="D9" t="n">
-        <v>19.70979510566992</v>
+        <v>18.01042987056885</v>
       </c>
       <c r="E9" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="10">
@@ -601,16 +601,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2.036174337624066</v>
+        <v>1.989392448091735</v>
       </c>
       <c r="C10" t="n">
-        <v>5.010189282100506</v>
+        <v>5.011254249646172</v>
       </c>
       <c r="D10" t="n">
-        <v>19.7061135692603</v>
+        <v>18.0067525497877</v>
       </c>
       <c r="E10" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1.903299715709692</v>
+        <v>1.856501497959063</v>
       </c>
       <c r="C11" t="n">
-        <v>5.016833013196225</v>
+        <v>5.017898797152806</v>
       </c>
       <c r="D11" t="n">
-        <v>19.71009980791774</v>
+        <v>18.01073927829168</v>
       </c>
       <c r="E11" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="12">
@@ -635,16 +635,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2.316713139936135</v>
+        <v>2.269903865874106</v>
       </c>
       <c r="C12" t="n">
-        <v>4.996162341984903</v>
+        <v>4.997228678757054</v>
       </c>
       <c r="D12" t="n">
-        <v>19.69769740519094</v>
+        <v>17.99833720725423</v>
       </c>
       <c r="E12" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2.494730578904634</v>
+        <v>2.447936313142641</v>
       </c>
       <c r="C13" t="n">
-        <v>4.987261470036477</v>
+        <v>4.988327056393627</v>
       </c>
       <c r="D13" t="n">
-        <v>19.69235688202189</v>
+        <v>17.99299623383618</v>
       </c>
       <c r="E13" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="14">
@@ -669,16 +669,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2.396151747336444</v>
+        <v>2.349364768306158</v>
       </c>
       <c r="C14" t="n">
-        <v>4.992190411614887</v>
+        <v>4.993255633635451</v>
       </c>
       <c r="D14" t="n">
-        <v>19.69531424696893</v>
+        <v>17.99595338018127</v>
       </c>
       <c r="E14" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="15">
@@ -686,16 +686,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.618572110199211</v>
+        <v>2.571803735167741</v>
       </c>
       <c r="C15" t="n">
-        <v>4.981069393471749</v>
+        <v>4.982133685292372</v>
       </c>
       <c r="D15" t="n">
-        <v>19.68864163608305</v>
+        <v>17.98928021117542</v>
       </c>
       <c r="E15" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="16">
@@ -703,16 +703,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.497550821010851</v>
+        <v>2.450790398225022</v>
       </c>
       <c r="C16" t="n">
-        <v>4.987120457931167</v>
+        <v>4.988184352139508</v>
       </c>
       <c r="D16" t="n">
-        <v>19.6922722747587</v>
+        <v>17.9929106112837</v>
       </c>
       <c r="E16" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="17">
@@ -720,16 +720,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.224165786784055</v>
+        <v>2.177408003559448</v>
       </c>
       <c r="C17" t="n">
-        <v>5.000789709642507</v>
+        <v>5.001853471872787</v>
       </c>
       <c r="D17" t="n">
-        <v>19.7004738257855</v>
+        <v>18.00111208312367</v>
       </c>
       <c r="E17" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="18">
@@ -737,16 +737,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.196144498833175</v>
+        <v>2.149392733856007</v>
       </c>
       <c r="C18" t="n">
-        <v>5.00219077404005</v>
+        <v>5.003254235357959</v>
       </c>
       <c r="D18" t="n">
-        <v>19.70131446442403</v>
+        <v>18.00195254121477</v>
       </c>
       <c r="E18" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="19">
@@ -754,16 +754,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1.995100181696944</v>
+        <v>1.948349470745689</v>
       </c>
       <c r="C19" t="n">
-        <v>5.012242989896862</v>
+        <v>5.013306398513475</v>
       </c>
       <c r="D19" t="n">
-        <v>19.70734579393812</v>
+        <v>18.00798383910809</v>
       </c>
       <c r="E19" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="20">
@@ -771,16 +771,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.325769331515044</v>
+        <v>2.279020965528495</v>
       </c>
       <c r="C20" t="n">
-        <v>4.995709532405957</v>
+        <v>4.996772823774334</v>
       </c>
       <c r="D20" t="n">
-        <v>19.69742571944357</v>
+        <v>17.9980636942646</v>
       </c>
       <c r="E20" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="21">
@@ -788,16 +788,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2.187123180971578</v>
+        <v>2.14037559436109</v>
       </c>
       <c r="C21" t="n">
-        <v>5.002641839933131</v>
+        <v>5.003705092332704</v>
       </c>
       <c r="D21" t="n">
-        <v>19.70158510395988</v>
+        <v>18.00222305539962</v>
       </c>
       <c r="E21" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="22">
@@ -805,16 +805,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>2.081518319590787</v>
+        <v>2.034771198281994</v>
       </c>
       <c r="C22" t="n">
-        <v>5.00792208300217</v>
+        <v>5.00898531213666</v>
       </c>
       <c r="D22" t="n">
-        <v>19.7047532498013</v>
+        <v>18.00539118728199</v>
       </c>
       <c r="E22" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="23">
@@ -822,16 +822,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1.967361163133842</v>
+        <v>1.920614179480678</v>
       </c>
       <c r="C23" t="n">
-        <v>5.013629940825017</v>
+        <v>5.014693163076725</v>
       </c>
       <c r="D23" t="n">
-        <v>19.70817796449501</v>
+        <v>18.00881589784603</v>
       </c>
       <c r="E23" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="24">
@@ -839,16 +839,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2.478555732954657</v>
+        <v>2.431809048662672</v>
       </c>
       <c r="C24" t="n">
-        <v>4.988070212333977</v>
+        <v>4.989133419617626</v>
       </c>
       <c r="D24" t="n">
-        <v>19.69284212740039</v>
+        <v>17.99348005177058</v>
       </c>
       <c r="E24" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="25">
@@ -856,16 +856,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2.343406366850301</v>
+        <v>2.296659729759078</v>
       </c>
       <c r="C25" t="n">
-        <v>4.994827680639195</v>
+        <v>4.995890885562805</v>
       </c>
       <c r="D25" t="n">
-        <v>19.69689660838351</v>
+        <v>17.99753453133768</v>
       </c>
       <c r="E25" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="26">
@@ -873,16 +873,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2.170872610009173</v>
+        <v>2.124126023932716</v>
       </c>
       <c r="C26" t="n">
-        <v>5.00345436848125</v>
+        <v>5.004517570854123</v>
       </c>
       <c r="D26" t="n">
-        <v>19.70207262108875</v>
+        <v>18.00271054251247</v>
       </c>
       <c r="E26" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="27">
@@ -890,16 +890,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>2.057393088050168</v>
+        <v>2.010646543334365</v>
       </c>
       <c r="C27" t="n">
-        <v>5.009128344579201</v>
+        <v>5.010191544884041</v>
       </c>
       <c r="D27" t="n">
-        <v>19.70547700674752</v>
+        <v>18.00611492693043</v>
       </c>
       <c r="E27" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +907,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>2.254926001460368</v>
+        <v>2.208179516372375</v>
       </c>
       <c r="C28" t="n">
-        <v>4.999251698908691</v>
+        <v>5.00031489623214</v>
       </c>
       <c r="D28" t="n">
-        <v>19.69955101934521</v>
+        <v>18.00018893773928</v>
       </c>
       <c r="E28" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="29">
@@ -924,16 +924,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>2.31526670961052</v>
+        <v>2.268520235013024</v>
       </c>
       <c r="C29" t="n">
-        <v>4.996234663501183</v>
+        <v>4.997297860300108</v>
       </c>
       <c r="D29" t="n">
-        <v>19.69774079810071</v>
+        <v>17.99837871618006</v>
       </c>
       <c r="E29" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="30">
@@ -941,16 +941,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>2.356926863132273</v>
+        <v>2.310180394542469</v>
       </c>
       <c r="C30" t="n">
-        <v>4.994151655825096</v>
+        <v>4.995214852323635</v>
       </c>
       <c r="D30" t="n">
-        <v>19.69649099349506</v>
+        <v>17.99712891139418</v>
       </c>
       <c r="E30" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="31">
@@ -958,16 +958,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>2.380214973194494</v>
+        <v>2.333468508036785</v>
       </c>
       <c r="C31" t="n">
-        <v>4.992987250321985</v>
+        <v>4.99405044664892</v>
       </c>
       <c r="D31" t="n">
-        <v>19.69579235019319</v>
+        <v>17.99643026798935</v>
       </c>
       <c r="E31" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="32">
@@ -975,16 +975,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>3.032703096888002</v>
+        <v>2.985956633686791</v>
       </c>
       <c r="C32" t="n">
-        <v>4.960362844137309</v>
+        <v>4.96142604036642</v>
       </c>
       <c r="D32" t="n">
-        <v>19.67621770648238</v>
+        <v>17.97685562421985</v>
       </c>
       <c r="E32" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="33">
@@ -992,16 +992,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>2.682776448450015</v>
+        <v>2.636029985805414</v>
       </c>
       <c r="C33" t="n">
-        <v>4.977859176559209</v>
+        <v>4.978922372760488</v>
       </c>
       <c r="D33" t="n">
-        <v>19.68671550593552</v>
+        <v>17.98735342365629</v>
       </c>
       <c r="E33" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="34">
@@ -1009,16 +1009,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>2.349435209406707</v>
+        <v>2.302688747356581</v>
       </c>
       <c r="C34" t="n">
-        <v>4.994526238511374</v>
+        <v>4.99558943468293</v>
       </c>
       <c r="D34" t="n">
-        <v>19.69671574310683</v>
+        <v>17.99735366080976</v>
       </c>
       <c r="E34" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="35">
@@ -1026,16 +1026,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>2.063399334111917</v>
+        <v>2.016652872538359</v>
       </c>
       <c r="C35" t="n">
-        <v>5.008828032276114</v>
+        <v>5.009891228423841</v>
       </c>
       <c r="D35" t="n">
-        <v>19.70529681936567</v>
+        <v>18.0059347370543</v>
       </c>
       <c r="E35" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="36">
@@ -1043,16 +1043,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>2.220474434187422</v>
+        <v>2.17372797329359</v>
       </c>
       <c r="C36" t="n">
-        <v>5.000974277272339</v>
+        <v>5.002037473386079</v>
       </c>
       <c r="D36" t="n">
-        <v>19.7005845663634</v>
+        <v>18.00122248403165</v>
       </c>
       <c r="E36" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="37">
@@ -1060,16 +1060,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2.588719740435256</v>
+        <v>2.541973279656366</v>
       </c>
       <c r="C37" t="n">
-        <v>4.982562011959947</v>
+        <v>4.983625208067941</v>
       </c>
       <c r="D37" t="n">
-        <v>19.68953720717597</v>
+        <v>17.99017512484076</v>
       </c>
       <c r="E37" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>2.427916323600179</v>
+        <v>2.381169862853769</v>
       </c>
       <c r="C38" t="n">
-        <v>4.990602182801701</v>
+        <v>4.99166537890807</v>
       </c>
       <c r="D38" t="n">
-        <v>19.69436130968102</v>
+        <v>17.99499922734484</v>
       </c>
       <c r="E38" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2.147349678878081</v>
+        <v>2.100603218166251</v>
       </c>
       <c r="C39" t="n">
-        <v>5.004630515037805</v>
+        <v>5.005693711142446</v>
       </c>
       <c r="D39" t="n">
-        <v>19.70277830902268</v>
+        <v>18.00341622668547</v>
       </c>
       <c r="E39" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="40">
@@ -1111,16 +1111,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>1.930798724462055</v>
+        <v>1.884052263777862</v>
       </c>
       <c r="C40" t="n">
-        <v>5.015458062758607</v>
+        <v>5.016521258861866</v>
       </c>
       <c r="D40" t="n">
-        <v>19.70927483765516</v>
+        <v>18.00991275531712</v>
       </c>
       <c r="E40" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1128,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>2.208511265302606</v>
+        <v>2.161764804657714</v>
       </c>
       <c r="C41" t="n">
-        <v>5.001572435716579</v>
+        <v>5.002635631817873</v>
       </c>
       <c r="D41" t="n">
-        <v>19.70094346142995</v>
+        <v>18.00158137909072</v>
       </c>
       <c r="E41" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="42">
@@ -1145,16 +1145,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>2.438955088243986</v>
+        <v>2.392208627605666</v>
       </c>
       <c r="C42" t="n">
-        <v>4.990050244569511</v>
+        <v>4.991113440670476</v>
       </c>
       <c r="D42" t="n">
-        <v>19.69403014674171</v>
+        <v>17.99466806440229</v>
       </c>
       <c r="E42" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="43">
@@ -1162,16 +1162,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>2.454914744017297</v>
+        <v>2.408168283382676</v>
       </c>
       <c r="C43" t="n">
-        <v>4.989252261780845</v>
+        <v>4.990315457881625</v>
       </c>
       <c r="D43" t="n">
-        <v>19.69355135706851</v>
+        <v>17.99418927472897</v>
       </c>
       <c r="E43" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="44">
@@ -1179,16 +1179,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>2.230843505805499</v>
+        <v>2.184097045171919</v>
       </c>
       <c r="C44" t="n">
-        <v>5.000455823691435</v>
+        <v>5.001519019792163</v>
       </c>
       <c r="D44" t="n">
-        <v>19.70027349421486</v>
+        <v>18.0009114118753</v>
       </c>
       <c r="E44" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1196,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>2.166946323049789</v>
+        <v>2.120199862418421</v>
       </c>
       <c r="C45" t="n">
-        <v>5.00365068282922</v>
+        <v>5.004713878929838</v>
       </c>
       <c r="D45" t="n">
-        <v>19.70219040969753</v>
+        <v>18.0028283273579</v>
       </c>
       <c r="E45" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="46">
@@ -1213,16 +1213,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>2.186915785886805</v>
+        <v>2.140169325256095</v>
       </c>
       <c r="C46" t="n">
-        <v>5.002652209687369</v>
+        <v>5.003715405787954</v>
       </c>
       <c r="D46" t="n">
-        <v>19.70159132581242</v>
+        <v>18.00222924347277</v>
       </c>
       <c r="E46" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1230,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>2.233171747945063</v>
+        <v>2.186425287314723</v>
       </c>
       <c r="C47" t="n">
-        <v>5.000339411584457</v>
+        <v>5.001402607685023</v>
       </c>
       <c r="D47" t="n">
-        <v>19.70020364695067</v>
+        <v>18.00084156461102</v>
       </c>
       <c r="E47" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1247,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>2.496908126624085</v>
+        <v>2.450161665993952</v>
       </c>
       <c r="C48" t="n">
-        <v>4.987152592650506</v>
+        <v>4.988215788751061</v>
       </c>
       <c r="D48" t="n">
-        <v>19.6922915555903</v>
+        <v>17.99292947325064</v>
       </c>
       <c r="E48" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1264,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>2.35769516979095</v>
+        <v>2.310948709160934</v>
       </c>
       <c r="C49" t="n">
-        <v>4.994113240492162</v>
+        <v>4.995176436592712</v>
       </c>
       <c r="D49" t="n">
-        <v>19.6964679442953</v>
+        <v>17.99710586195563</v>
       </c>
       <c r="E49" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="50">
@@ -1281,16 +1281,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>2.47380199501432</v>
+        <v>2.427055534384369</v>
       </c>
       <c r="C50" t="n">
-        <v>4.988307899230993</v>
+        <v>4.98937109533154</v>
       </c>
       <c r="D50" t="n">
-        <v>19.69298473953859</v>
+        <v>17.99362265719892</v>
       </c>
       <c r="E50" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
     <row r="51">
@@ -1298,186 +1298,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>2.381845346496632</v>
+        <v>2.335098885866699</v>
       </c>
       <c r="C51" t="n">
-        <v>4.992905731656878</v>
+        <v>4.993968927757424</v>
       </c>
       <c r="D51" t="n">
-        <v>19.69574343899412</v>
+        <v>17.99638135665445</v>
       </c>
       <c r="E51" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>51</v>
-      </c>
-      <c r="B52" t="n">
-        <v>2.300404952582564</v>
-      </c>
-      <c r="C52" t="n">
-        <v>4.996977751352581</v>
-      </c>
-      <c r="D52" t="n">
-        <v>19.69818665081155</v>
-      </c>
-      <c r="E52" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" t="n">
-        <v>2.433222429889164</v>
-      </c>
-      <c r="C53" t="n">
-        <v>4.990336877487251</v>
-      </c>
-      <c r="D53" t="n">
-        <v>19.69420212649235</v>
-      </c>
-      <c r="E53" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" t="n">
-        <v>2.066875287975035</v>
-      </c>
-      <c r="C54" t="n">
-        <v>5.008654234582957</v>
-      </c>
-      <c r="D54" t="n">
-        <v>19.70519254074977</v>
-      </c>
-      <c r="E54" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" t="n">
-        <v>1.95256857547008</v>
-      </c>
-      <c r="C55" t="n">
-        <v>5.014369570208205</v>
-      </c>
-      <c r="D55" t="n">
-        <v>19.70862174212492</v>
-      </c>
-      <c r="E55" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>55</v>
-      </c>
-      <c r="B56" t="n">
-        <v>1.836105668098958</v>
-      </c>
-      <c r="C56" t="n">
-        <v>5.020192715576761</v>
-      </c>
-      <c r="D56" t="n">
-        <v>19.71211562934606</v>
-      </c>
-      <c r="E56" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>56</v>
-      </c>
-      <c r="B57" t="n">
-        <v>1.771894296844883</v>
-      </c>
-      <c r="C57" t="n">
-        <v>5.023403284139465</v>
-      </c>
-      <c r="D57" t="n">
-        <v>19.71404197048368</v>
-      </c>
-      <c r="E57" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>57</v>
-      </c>
-      <c r="B58" t="n">
-        <v>1.883247692517815</v>
-      </c>
-      <c r="C58" t="n">
-        <v>5.017835614355818</v>
-      </c>
-      <c r="D58" t="n">
-        <v>19.71070136861349</v>
-      </c>
-      <c r="E58" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>58</v>
-      </c>
-      <c r="B59" t="n">
-        <v>2.592868008508101</v>
-      </c>
-      <c r="C59" t="n">
-        <v>4.982354598556304</v>
-      </c>
-      <c r="D59" t="n">
-        <v>19.68941275913378</v>
-      </c>
-      <c r="E59" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>59</v>
-      </c>
-      <c r="B60" t="n">
-        <v>2.289456912338108</v>
-      </c>
-      <c r="C60" t="n">
-        <v>4.997525153364804</v>
-      </c>
-      <c r="D60" t="n">
-        <v>19.69851509201888</v>
-      </c>
-      <c r="E60" t="n">
-        <v>2.239959979634188</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>60</v>
-      </c>
-      <c r="B61" t="n">
-        <v>2.43552439248799</v>
-      </c>
-      <c r="C61" t="n">
-        <v>4.99022177935731</v>
-      </c>
-      <c r="D61" t="n">
-        <v>19.69413306761438</v>
-      </c>
-      <c r="E61" t="n">
-        <v>2.239959979634188</v>
+        <v>2.21447744101518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified files and app for poly model
</commit_message>
<xml_diff>
--- a/data/constant_height_profile.xlsx
+++ b/data/constant_height_profile.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.095160230104522</v>
+        <v>2.026832554851517</v>
       </c>
       <c r="C2" t="n">
-        <v>5.005965860545533</v>
+        <v>7.007617129875967</v>
       </c>
       <c r="D2" t="n">
-        <v>18.00357951632732</v>
+        <v>14.50457027792558</v>
       </c>
       <c r="E2" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1.886232637392391</v>
+        <v>1.848290115949497</v>
       </c>
       <c r="C3" t="n">
-        <v>5.01641224018114</v>
+        <v>7.016544251821068</v>
       </c>
       <c r="D3" t="n">
-        <v>18.00984734410869</v>
+        <v>14.50992655109264</v>
       </c>
       <c r="E3" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.19309545946011</v>
+        <v>2.214740153395388</v>
       </c>
       <c r="C4" t="n">
-        <v>5.001069099077753</v>
+        <v>6.998221749948773</v>
       </c>
       <c r="D4" t="n">
-        <v>18.00064145944665</v>
+        <v>14.49893304996926</v>
       </c>
       <c r="E4" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2.473148346168887</v>
+        <v>2.508657445398764</v>
       </c>
       <c r="C5" t="n">
-        <v>4.987066454742314</v>
+        <v>6.983525885348604</v>
       </c>
       <c r="D5" t="n">
-        <v>17.99223987284539</v>
+        <v>14.49011553120916</v>
       </c>
       <c r="E5" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1.986185746177197</v>
+        <v>2.024935625639178</v>
       </c>
       <c r="C6" t="n">
-        <v>5.011414584741899</v>
+        <v>7.007711976336584</v>
       </c>
       <c r="D6" t="n">
-        <v>18.00684875084514</v>
+        <v>14.50462718580195</v>
       </c>
       <c r="E6" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +550,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1.672671793337828</v>
+        <v>1.714526462615308</v>
       </c>
       <c r="C7" t="n">
-        <v>5.027090282383868</v>
+        <v>7.023232434487777</v>
       </c>
       <c r="D7" t="n">
-        <v>18.01625416943032</v>
+        <v>14.51393946069267</v>
       </c>
       <c r="E7" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +567,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.842194708816258</v>
+        <v>1.888476163776437</v>
       </c>
       <c r="C8" t="n">
-        <v>5.018614136609946</v>
+        <v>7.014534949429721</v>
       </c>
       <c r="D8" t="n">
-        <v>18.01116848196597</v>
+        <v>14.50872096965783</v>
       </c>
       <c r="E8" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="9">
@@ -584,16 +584,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>1.866815088720299</v>
+        <v>1.913661403078272</v>
       </c>
       <c r="C9" t="n">
-        <v>5.017383117614744</v>
+        <v>7.013275687464629</v>
       </c>
       <c r="D9" t="n">
-        <v>18.01042987056885</v>
+        <v>14.50796541247878</v>
       </c>
       <c r="E9" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="10">
@@ -601,16 +601,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1.989392448091735</v>
+        <v>2.036464684285316</v>
       </c>
       <c r="C10" t="n">
-        <v>5.011254249646172</v>
+        <v>7.007135523404277</v>
       </c>
       <c r="D10" t="n">
-        <v>18.0067525497877</v>
+        <v>14.50428131404257</v>
       </c>
       <c r="E10" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1.856501497959063</v>
+        <v>1.903613705942842</v>
       </c>
       <c r="C11" t="n">
-        <v>5.017898797152806</v>
+        <v>7.013778072321401</v>
       </c>
       <c r="D11" t="n">
-        <v>18.01073927829168</v>
+        <v>14.50826684339284</v>
       </c>
       <c r="E11" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="12">
@@ -635,16 +635,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2.269903865874106</v>
+        <v>2.31707682200459</v>
       </c>
       <c r="C12" t="n">
-        <v>4.997228678757054</v>
+        <v>6.993104916518313</v>
       </c>
       <c r="D12" t="n">
-        <v>17.99833720725423</v>
+        <v>14.49586294991099</v>
       </c>
       <c r="E12" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2.447936313142641</v>
+        <v>2.495108545344365</v>
       </c>
       <c r="C13" t="n">
-        <v>4.988327056393627</v>
+        <v>6.984203330351324</v>
       </c>
       <c r="D13" t="n">
-        <v>17.99299623383618</v>
+        <v>14.4905219982108</v>
       </c>
       <c r="E13" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="14">
@@ -669,16 +669,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2.349364768306158</v>
+        <v>2.396533614978456</v>
       </c>
       <c r="C14" t="n">
-        <v>4.993255633635451</v>
+        <v>6.98913207686962</v>
       </c>
       <c r="D14" t="n">
-        <v>17.99595338018127</v>
+        <v>14.49347924612177</v>
       </c>
       <c r="E14" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="15">
@@ -686,16 +686,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.571803735167741</v>
+        <v>2.618962126001942</v>
       </c>
       <c r="C15" t="n">
-        <v>4.982133685292372</v>
+        <v>6.978010651318446</v>
       </c>
       <c r="D15" t="n">
-        <v>17.98928021117542</v>
+        <v>14.48680639079107</v>
       </c>
       <c r="E15" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="16">
@@ -703,16 +703,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.450790398225022</v>
+        <v>2.497943141303671</v>
       </c>
       <c r="C16" t="n">
-        <v>4.988184352139508</v>
+        <v>6.984061600553359</v>
       </c>
       <c r="D16" t="n">
-        <v>17.9929106112837</v>
+        <v>14.49043696033202</v>
       </c>
       <c r="E16" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="17">
@@ -720,16 +720,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.177408003559448</v>
+        <v>2.224558730565484</v>
       </c>
       <c r="C17" t="n">
-        <v>5.001853471872787</v>
+        <v>6.997730821090268</v>
       </c>
       <c r="D17" t="n">
-        <v>18.00111208312367</v>
+        <v>14.49863849265416</v>
       </c>
       <c r="E17" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="18">
@@ -737,16 +737,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.149392733856007</v>
+        <v>2.19653873915436</v>
       </c>
       <c r="C18" t="n">
-        <v>5.003254235357959</v>
+        <v>6.999131820660825</v>
       </c>
       <c r="D18" t="n">
-        <v>18.00195254121477</v>
+        <v>14.49947909239649</v>
       </c>
       <c r="E18" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="19">
@@ -754,16 +754,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1.948349470745689</v>
+        <v>1.995494603242188</v>
       </c>
       <c r="C19" t="n">
-        <v>5.013306398513475</v>
+        <v>7.009184027456433</v>
       </c>
       <c r="D19" t="n">
-        <v>18.00798383910809</v>
+        <v>14.50551041647386</v>
       </c>
       <c r="E19" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="20">
@@ -771,16 +771,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.279020965528495</v>
+        <v>2.326164129062615</v>
       </c>
       <c r="C20" t="n">
-        <v>4.996772823774334</v>
+        <v>6.992650551165412</v>
       </c>
       <c r="D20" t="n">
-        <v>17.9980636942646</v>
+        <v>14.49559033069925</v>
       </c>
       <c r="E20" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="21">
@@ -788,16 +788,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2.14037559436109</v>
+        <v>2.187518082993412</v>
       </c>
       <c r="C21" t="n">
-        <v>5.003705092332704</v>
+        <v>6.999582853468872</v>
       </c>
       <c r="D21" t="n">
-        <v>18.00222305539962</v>
+        <v>14.49974971208132</v>
       </c>
       <c r="E21" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="22">
@@ -805,16 +805,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>2.034771198281994</v>
+        <v>2.081913277552314</v>
       </c>
       <c r="C22" t="n">
-        <v>5.00898531213666</v>
+        <v>7.004863093740926</v>
       </c>
       <c r="D22" t="n">
-        <v>18.00539118728199</v>
+        <v>14.50291785624456</v>
       </c>
       <c r="E22" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="23">
@@ -822,16 +822,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1.920614179480678</v>
+        <v>1.967756136047482</v>
       </c>
       <c r="C23" t="n">
-        <v>5.014693163076725</v>
+        <v>7.010570950816168</v>
       </c>
       <c r="D23" t="n">
-        <v>18.00881589784603</v>
+        <v>14.5063425704897</v>
       </c>
       <c r="E23" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="24">
@@ -839,16 +839,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2.431809048662672</v>
+        <v>2.478950736782869</v>
       </c>
       <c r="C24" t="n">
-        <v>4.989133419617626</v>
+        <v>6.985011220779399</v>
       </c>
       <c r="D24" t="n">
-        <v>17.99348005177058</v>
+        <v>14.49100673246764</v>
       </c>
       <c r="E24" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="25">
@@ -856,16 +856,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2.296659729759078</v>
+        <v>2.343801374932919</v>
       </c>
       <c r="C25" t="n">
-        <v>4.995890885562805</v>
+        <v>6.991768688871897</v>
       </c>
       <c r="D25" t="n">
-        <v>17.99753453133768</v>
+        <v>14.49506121332314</v>
       </c>
       <c r="E25" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="26">
@@ -873,16 +873,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2.124126023932716</v>
+        <v>2.17126762248391</v>
       </c>
       <c r="C26" t="n">
-        <v>5.004517570854123</v>
+        <v>7.000395376494347</v>
       </c>
       <c r="D26" t="n">
-        <v>18.00271054251247</v>
+        <v>14.50023722589661</v>
       </c>
       <c r="E26" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="27">
@@ -890,16 +890,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>2.010646543334365</v>
+        <v>2.057788103925299</v>
       </c>
       <c r="C27" t="n">
-        <v>5.010191544884041</v>
+        <v>7.006069352422277</v>
       </c>
       <c r="D27" t="n">
-        <v>18.00611492693043</v>
+        <v>14.50364161145337</v>
       </c>
       <c r="E27" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +907,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>2.208179516372375</v>
+        <v>2.255321022015243</v>
       </c>
       <c r="C28" t="n">
-        <v>5.00031489623214</v>
+        <v>6.99619270651778</v>
       </c>
       <c r="D28" t="n">
-        <v>18.00018893773928</v>
+        <v>14.49771562391067</v>
       </c>
       <c r="E28" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="29">
@@ -924,16 +924,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>2.268520235013024</v>
+        <v>2.315661730844203</v>
       </c>
       <c r="C29" t="n">
-        <v>4.997297860300108</v>
+        <v>6.993175671076332</v>
       </c>
       <c r="D29" t="n">
-        <v>17.99837871618006</v>
+        <v>14.4959054026458</v>
       </c>
       <c r="E29" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="30">
@@ -941,16 +941,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>2.310180394542469</v>
+        <v>2.357321884725773</v>
       </c>
       <c r="C30" t="n">
-        <v>4.995214852323635</v>
+        <v>6.991092663382254</v>
       </c>
       <c r="D30" t="n">
-        <v>17.99712891139418</v>
+        <v>14.49465559802935</v>
       </c>
       <c r="E30" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="31">
@@ -958,16 +958,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>2.333468508036785</v>
+        <v>2.380609994978547</v>
       </c>
       <c r="C31" t="n">
-        <v>4.99405044664892</v>
+        <v>6.989928257869615</v>
       </c>
       <c r="D31" t="n">
-        <v>17.99643026798935</v>
+        <v>14.49395695472177</v>
       </c>
       <c r="E31" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="32">
@@ -975,16 +975,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2.985956633686791</v>
+        <v>3.033098118772881</v>
       </c>
       <c r="C32" t="n">
-        <v>4.96142604036642</v>
+        <v>6.957303851679899</v>
       </c>
       <c r="D32" t="n">
-        <v>17.97685562421985</v>
+        <v>14.47438231100794</v>
       </c>
       <c r="E32" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="33">
@@ -992,16 +992,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>2.636029985805414</v>
+        <v>2.683171470361548</v>
       </c>
       <c r="C33" t="n">
-        <v>4.978922372760488</v>
+        <v>6.974800184100465</v>
       </c>
       <c r="D33" t="n">
-        <v>17.98735342365629</v>
+        <v>14.48488011046028</v>
       </c>
       <c r="E33" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="34">
@@ -1009,16 +1009,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>2.302688747356581</v>
+        <v>2.349830231345646</v>
       </c>
       <c r="C34" t="n">
-        <v>4.99558943468293</v>
+        <v>6.99146724605126</v>
       </c>
       <c r="D34" t="n">
-        <v>17.99735366080976</v>
+        <v>14.49488034763076</v>
       </c>
       <c r="E34" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="35">
@@ -1026,16 +1026,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>2.016652872538359</v>
+        <v>2.063794356071993</v>
       </c>
       <c r="C35" t="n">
-        <v>5.009891228423841</v>
+        <v>7.005769039814943</v>
       </c>
       <c r="D35" t="n">
-        <v>18.0059347370543</v>
+        <v>14.50346142388897</v>
       </c>
       <c r="E35" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="36">
@@ -1043,16 +1043,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>2.17372797329359</v>
+        <v>2.220869456176477</v>
       </c>
       <c r="C36" t="n">
-        <v>5.002037473386079</v>
+        <v>6.997915284809719</v>
       </c>
       <c r="D36" t="n">
-        <v>18.00122248403165</v>
+        <v>14.49874917088583</v>
       </c>
       <c r="E36" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="37">
@@ -1060,16 +1060,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2.541973279656366</v>
+        <v>2.589114762428446</v>
       </c>
       <c r="C37" t="n">
-        <v>4.983625208067941</v>
+        <v>6.979503019497121</v>
       </c>
       <c r="D37" t="n">
-        <v>17.99017512484076</v>
+        <v>14.48770181169827</v>
       </c>
       <c r="E37" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>2.381169862853769</v>
+        <v>2.428311345594457</v>
       </c>
       <c r="C38" t="n">
-        <v>4.99166537890807</v>
+        <v>6.98754319033882</v>
       </c>
       <c r="D38" t="n">
-        <v>17.99499922734484</v>
+        <v>14.49252591420329</v>
       </c>
       <c r="E38" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2.100603218166251</v>
+        <v>2.147744700873476</v>
       </c>
       <c r="C39" t="n">
-        <v>5.005693711142446</v>
+        <v>7.001571522574869</v>
       </c>
       <c r="D39" t="n">
-        <v>18.00341622668547</v>
+        <v>14.50094291354492</v>
       </c>
       <c r="E39" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="40">
@@ -1111,16 +1111,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>1.884052263777862</v>
+        <v>1.931193746458312</v>
       </c>
       <c r="C40" t="n">
-        <v>5.016521258861866</v>
+        <v>7.012399070295627</v>
       </c>
       <c r="D40" t="n">
-        <v>18.00991275531712</v>
+        <v>14.50743944217738</v>
       </c>
       <c r="E40" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1128,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>2.161764804657714</v>
+        <v>2.208906287300041</v>
       </c>
       <c r="C41" t="n">
-        <v>5.002635631817873</v>
+        <v>6.998513443253541</v>
       </c>
       <c r="D41" t="n">
-        <v>18.00158137909072</v>
+        <v>14.49910806595213</v>
       </c>
       <c r="E41" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="42">
@@ -1145,16 +1145,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>2.392208627605666</v>
+        <v>2.439350110241588</v>
       </c>
       <c r="C42" t="n">
-        <v>4.991113440670476</v>
+        <v>6.986991252106463</v>
       </c>
       <c r="D42" t="n">
-        <v>17.99466806440229</v>
+        <v>14.49219475126388</v>
       </c>
       <c r="E42" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="43">
@@ -1162,16 +1162,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>2.408168283382676</v>
+        <v>2.455309766014986</v>
       </c>
       <c r="C43" t="n">
-        <v>4.990315457881625</v>
+        <v>6.986193269317793</v>
       </c>
       <c r="D43" t="n">
-        <v>17.99418927472897</v>
+        <v>14.49171596159068</v>
       </c>
       <c r="E43" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="44">
@@ -1179,16 +1179,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>2.184097045171919</v>
+        <v>2.231238527803211</v>
       </c>
       <c r="C44" t="n">
-        <v>5.001519019792163</v>
+        <v>6.997396831228382</v>
       </c>
       <c r="D44" t="n">
-        <v>18.0009114118753</v>
+        <v>14.49843809873703</v>
       </c>
       <c r="E44" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1196,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>2.120199862418421</v>
+        <v>2.167341345047549</v>
       </c>
       <c r="C45" t="n">
-        <v>5.004713878929838</v>
+        <v>7.000591690366165</v>
       </c>
       <c r="D45" t="n">
-        <v>18.0028283273579</v>
+        <v>14.5003550142197</v>
       </c>
       <c r="E45" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="46">
@@ -1213,16 +1213,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>2.140169325256095</v>
+        <v>2.187310807884578</v>
       </c>
       <c r="C46" t="n">
-        <v>5.003715405787954</v>
+        <v>6.999593217224314</v>
       </c>
       <c r="D46" t="n">
-        <v>18.00222924347277</v>
+        <v>14.49975593033459</v>
       </c>
       <c r="E46" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1230,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>2.186425287314723</v>
+        <v>2.233566769942843</v>
       </c>
       <c r="C47" t="n">
-        <v>5.001402607685023</v>
+        <v>6.997280419121401</v>
       </c>
       <c r="D47" t="n">
-        <v>18.00084156461102</v>
+        <v>14.49836825147284</v>
       </c>
       <c r="E47" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1247,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>2.450161665993952</v>
+        <v>2.497303148621868</v>
       </c>
       <c r="C48" t="n">
-        <v>4.988215788751061</v>
+        <v>6.984093600187449</v>
       </c>
       <c r="D48" t="n">
-        <v>17.99292947325064</v>
+        <v>14.49045616011247</v>
       </c>
       <c r="E48" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1264,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>2.310948709160934</v>
+        <v>2.358090191788734</v>
       </c>
       <c r="C49" t="n">
-        <v>4.995176436592712</v>
+        <v>6.991054248029106</v>
       </c>
       <c r="D49" t="n">
-        <v>17.99710586195563</v>
+        <v>14.49463254881746</v>
       </c>
       <c r="E49" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="50">
@@ -1281,16 +1281,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>2.427055534384369</v>
+        <v>2.474197017012105</v>
       </c>
       <c r="C50" t="n">
-        <v>4.98937109533154</v>
+        <v>6.985248906767938</v>
       </c>
       <c r="D50" t="n">
-        <v>17.99362265719892</v>
+        <v>14.49114934406076</v>
       </c>
       <c r="E50" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
       </c>
     </row>
     <row r="51">
@@ -1298,16 +1298,866 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>2.335098885866699</v>
+        <v>2.382240368494418</v>
       </c>
       <c r="C51" t="n">
-        <v>4.993968927757424</v>
+        <v>6.989846739193822</v>
       </c>
       <c r="D51" t="n">
-        <v>17.99638135665445</v>
+        <v>14.49390804351629</v>
       </c>
       <c r="E51" t="n">
-        <v>2.21447744101518</v>
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2.30079997458035</v>
+      </c>
+      <c r="C52" t="n">
+        <v>6.993918758889525</v>
+      </c>
+      <c r="D52" t="n">
+        <v>14.49635125533372</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2.433617451886951</v>
+      </c>
+      <c r="C53" t="n">
+        <v>6.987277885024195</v>
+      </c>
+      <c r="D53" t="n">
+        <v>14.49236673101452</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2.067270309972822</v>
+      </c>
+      <c r="C54" t="n">
+        <v>7.005595242119901</v>
+      </c>
+      <c r="D54" t="n">
+        <v>14.50335714527194</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.952963597467867</v>
+      </c>
+      <c r="C55" t="n">
+        <v>7.011310577745149</v>
+      </c>
+      <c r="D55" t="n">
+        <v>14.50678634664709</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.836500690096745</v>
+      </c>
+      <c r="C56" t="n">
+        <v>7.017133723113705</v>
+      </c>
+      <c r="D56" t="n">
+        <v>14.51028023386822</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.77228931884267</v>
+      </c>
+      <c r="C57" t="n">
+        <v>7.020344291676409</v>
+      </c>
+      <c r="D57" t="n">
+        <v>14.51220657500584</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.883642714515602</v>
+      </c>
+      <c r="C58" t="n">
+        <v>7.014776621892763</v>
+      </c>
+      <c r="D58" t="n">
+        <v>14.50886597313566</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.593263030505888</v>
+      </c>
+      <c r="C59" t="n">
+        <v>6.979295606093248</v>
+      </c>
+      <c r="D59" t="n">
+        <v>14.48757736365595</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.289851934335895</v>
+      </c>
+      <c r="C60" t="n">
+        <v>6.994466160901748</v>
+      </c>
+      <c r="D60" t="n">
+        <v>14.49667969654105</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.435919414485777</v>
+      </c>
+      <c r="C61" t="n">
+        <v>6.987162786894253</v>
+      </c>
+      <c r="D61" t="n">
+        <v>14.49229767213655</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.026442490486163</v>
+      </c>
+      <c r="C62" t="n">
+        <v>7.007636633094235</v>
+      </c>
+      <c r="D62" t="n">
+        <v>14.50458197985654</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.91307651942818</v>
+      </c>
+      <c r="C63" t="n">
+        <v>7.013304931647133</v>
+      </c>
+      <c r="D63" t="n">
+        <v>14.50798295898828</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.059143500951829</v>
+      </c>
+      <c r="C64" t="n">
+        <v>7.006001582570951</v>
+      </c>
+      <c r="D64" t="n">
+        <v>14.50360094954257</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2.32103792589358</v>
+      </c>
+      <c r="C65" t="n">
+        <v>6.992906861323863</v>
+      </c>
+      <c r="D65" t="n">
+        <v>14.49574411679432</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>2.471683425676749</v>
+      </c>
+      <c r="C66" t="n">
+        <v>6.985374586334705</v>
+      </c>
+      <c r="D66" t="n">
+        <v>14.49122475180082</v>
+      </c>
+      <c r="E66" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2.562178285869165</v>
+      </c>
+      <c r="C67" t="n">
+        <v>6.980849843325085</v>
+      </c>
+      <c r="D67" t="n">
+        <v>14.48850990599505</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2.365374828955619</v>
+      </c>
+      <c r="C68" t="n">
+        <v>6.990690016170761</v>
+      </c>
+      <c r="D68" t="n">
+        <v>14.49441400970246</v>
+      </c>
+      <c r="E68" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>2.167726946992427</v>
+      </c>
+      <c r="C69" t="n">
+        <v>7.000572410268921</v>
+      </c>
+      <c r="D69" t="n">
+        <v>14.50034344616135</v>
+      </c>
+      <c r="E69" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>2.387970495903073</v>
+      </c>
+      <c r="C70" t="n">
+        <v>6.989560232823389</v>
+      </c>
+      <c r="D70" t="n">
+        <v>14.49373613969403</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2.273395019205681</v>
+      </c>
+      <c r="C71" t="n">
+        <v>6.995289006658258</v>
+      </c>
+      <c r="D71" t="n">
+        <v>14.49717340399495</v>
+      </c>
+      <c r="E71" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.966900254457118</v>
+      </c>
+      <c r="C72" t="n">
+        <v>7.010613744895687</v>
+      </c>
+      <c r="D72" t="n">
+        <v>14.50636824693741</v>
+      </c>
+      <c r="E72" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1.741801126641431</v>
+      </c>
+      <c r="C73" t="n">
+        <v>7.021868701286471</v>
+      </c>
+      <c r="D73" t="n">
+        <v>14.51312122077188</v>
+      </c>
+      <c r="E73" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.641017518429263</v>
+      </c>
+      <c r="C74" t="n">
+        <v>7.026907881697079</v>
+      </c>
+      <c r="D74" t="n">
+        <v>14.51614472901825</v>
+      </c>
+      <c r="E74" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.082194020986123</v>
+      </c>
+      <c r="C75" t="n">
+        <v>7.004849056569237</v>
+      </c>
+      <c r="D75" t="n">
+        <v>14.50290943394154</v>
+      </c>
+      <c r="E75" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2.16329227627756</v>
+      </c>
+      <c r="C76" t="n">
+        <v>7.000794143804664</v>
+      </c>
+      <c r="D76" t="n">
+        <v>14.5004764862828</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2.401457411779471</v>
+      </c>
+      <c r="C77" t="n">
+        <v>6.988885887029569</v>
+      </c>
+      <c r="D77" t="n">
+        <v>14.49333153221774</v>
+      </c>
+      <c r="E77" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2.23844881489625</v>
+      </c>
+      <c r="C78" t="n">
+        <v>6.99703631687373</v>
+      </c>
+      <c r="D78" t="n">
+        <v>14.49822179012424</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2.166678339692831</v>
+      </c>
+      <c r="C79" t="n">
+        <v>7.000624840633901</v>
+      </c>
+      <c r="D79" t="n">
+        <v>14.50037490438034</v>
+      </c>
+      <c r="E79" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2.378396886769317</v>
+      </c>
+      <c r="C80" t="n">
+        <v>6.990038913280077</v>
+      </c>
+      <c r="D80" t="n">
+        <v>14.49402334796805</v>
+      </c>
+      <c r="E80" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2.24452187768137</v>
+      </c>
+      <c r="C81" t="n">
+        <v>6.996732663734474</v>
+      </c>
+      <c r="D81" t="n">
+        <v>14.49803959824068</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2.292748013812606</v>
+      </c>
+      <c r="C82" t="n">
+        <v>6.994321356927912</v>
+      </c>
+      <c r="D82" t="n">
+        <v>14.49659281415675</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2.118464773263224</v>
+      </c>
+      <c r="C83" t="n">
+        <v>7.003035518955381</v>
+      </c>
+      <c r="D83" t="n">
+        <v>14.50182131137323</v>
+      </c>
+      <c r="E83" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2.018539211612989</v>
+      </c>
+      <c r="C84" t="n">
+        <v>7.008031797037893</v>
+      </c>
+      <c r="D84" t="n">
+        <v>14.50481907822274</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
+        <v>1.901470033929272</v>
+      </c>
+      <c r="C85" t="n">
+        <v>7.013885255922079</v>
+      </c>
+      <c r="D85" t="n">
+        <v>14.50833115355325</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1.745026371416948</v>
+      </c>
+      <c r="C86" t="n">
+        <v>7.021707439047695</v>
+      </c>
+      <c r="D86" t="n">
+        <v>14.51302446342862</v>
+      </c>
+      <c r="E86" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2.097497098345468</v>
+      </c>
+      <c r="C87" t="n">
+        <v>7.004083902701269</v>
+      </c>
+      <c r="D87" t="n">
+        <v>14.50245034162076</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2.01839887650832</v>
+      </c>
+      <c r="C88" t="n">
+        <v>7.008038813793126</v>
+      </c>
+      <c r="D88" t="n">
+        <v>14.50482328827588</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2.057888342935312</v>
+      </c>
+      <c r="C89" t="n">
+        <v>7.006064340471777</v>
+      </c>
+      <c r="D89" t="n">
+        <v>14.50363860428307</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="n">
+        <v>2.280882278711224</v>
+      </c>
+      <c r="C90" t="n">
+        <v>6.994914643682981</v>
+      </c>
+      <c r="D90" t="n">
+        <v>14.49694878620979</v>
+      </c>
+      <c r="E90" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2.356266319019776</v>
+      </c>
+      <c r="C91" t="n">
+        <v>6.991145441667554</v>
+      </c>
+      <c r="D91" t="n">
+        <v>14.49468726500053</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2.468388517923142</v>
+      </c>
+      <c r="C92" t="n">
+        <v>6.985539331722386</v>
+      </c>
+      <c r="D92" t="n">
+        <v>14.49132359903343</v>
+      </c>
+      <c r="E92" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="n">
+        <v>2.346966581013413</v>
+      </c>
+      <c r="C93" t="n">
+        <v>6.991610428567872</v>
+      </c>
+      <c r="D93" t="n">
+        <v>14.49496625714072</v>
+      </c>
+      <c r="E93" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2.177138378724927</v>
+      </c>
+      <c r="C94" t="n">
+        <v>7.000101838682296</v>
+      </c>
+      <c r="D94" t="n">
+        <v>14.50006110320938</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2.050130980672533</v>
+      </c>
+      <c r="C95" t="n">
+        <v>7.006452208584916</v>
+      </c>
+      <c r="D95" t="n">
+        <v>14.50387132515095</v>
+      </c>
+      <c r="E95" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="n">
+        <v>1.756371691455941</v>
+      </c>
+      <c r="C96" t="n">
+        <v>7.021140173045746</v>
+      </c>
+      <c r="D96" t="n">
+        <v>14.51268410382745</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="n">
+        <v>1.538399624957957</v>
+      </c>
+      <c r="C97" t="n">
+        <v>7.032038776370645</v>
+      </c>
+      <c r="D97" t="n">
+        <v>14.51922326582239</v>
+      </c>
+      <c r="E97" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1.424668668706767</v>
+      </c>
+      <c r="C98" t="n">
+        <v>7.037725324183204</v>
+      </c>
+      <c r="D98" t="n">
+        <v>14.52263519450992</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="n">
+        <v>1.429552601115612</v>
+      </c>
+      <c r="C99" t="n">
+        <v>7.037481127562762</v>
+      </c>
+      <c r="D99" t="n">
+        <v>14.52248867653766</v>
+      </c>
+      <c r="E99" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="n">
+        <v>2.001774877861993</v>
+      </c>
+      <c r="C100" t="n">
+        <v>7.008870013725443</v>
+      </c>
+      <c r="D100" t="n">
+        <v>14.50532200823527</v>
+      </c>
+      <c r="E100" t="n">
+        <v>2.179175152370851</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1.869614329326609</v>
+      </c>
+      <c r="C101" t="n">
+        <v>7.015478041152212</v>
+      </c>
+      <c r="D101" t="n">
+        <v>14.50928682469133</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2.179175152370851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>